<commit_message>
Actualización automática de datos TSLA + modelo
</commit_message>
<xml_diff>
--- a/src/proyecto_integrado_V/static/data/TSLA_dashboard_data.xlsx
+++ b/src/proyecto_integrado_V/static/data/TSLA_dashboard_data.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -480,8 +476,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>45047</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-05-01 00:00:00</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>161.83</v>
@@ -494,8 +492,10 @@
       <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45048</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-05-02 00:00:00</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>160.31</v>
@@ -512,8 +512,10 @@
       <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>45049</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-05-03 00:00:00</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>160.61</v>
@@ -530,8 +532,10 @@
       <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>45050</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-05-04 00:00:00</t>
+        </is>
       </c>
       <c r="B5" t="n">
         <v>161.2</v>
@@ -548,8 +552,10 @@
       <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>45051</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-05-05 00:00:00</t>
+        </is>
       </c>
       <c r="B6" t="n">
         <v>170.06</v>
@@ -566,8 +572,10 @@
       <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>45054</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-05-08 00:00:00</t>
+        </is>
       </c>
       <c r="B7" t="n">
         <v>171.79</v>
@@ -584,8 +592,10 @@
       <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>45055</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-05-09 00:00:00</t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>169.15</v>
@@ -606,8 +616,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>45056</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-05-10 00:00:00</t>
+        </is>
       </c>
       <c r="B9" t="n">
         <v>168.54</v>
@@ -630,8 +642,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>45057</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-05-11 00:00:00</t>
+        </is>
       </c>
       <c r="B10" t="n">
         <v>172.08</v>
@@ -654,8 +668,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>45058</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2023-05-12 00:00:00</t>
+        </is>
       </c>
       <c r="B11" t="n">
         <v>167.98</v>
@@ -678,8 +694,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
-        <v>45061</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2023-05-15 00:00:00</t>
+        </is>
       </c>
       <c r="B12" t="n">
         <v>166.35</v>
@@ -702,8 +720,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n">
-        <v>45062</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
       </c>
       <c r="B13" t="n">
         <v>166.52</v>
@@ -726,8 +746,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n">
-        <v>45063</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-05-17 00:00:00</t>
+        </is>
       </c>
       <c r="B14" t="n">
         <v>173.86</v>
@@ -750,8 +772,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n">
-        <v>45064</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2023-05-18 00:00:00</t>
+        </is>
       </c>
       <c r="B15" t="n">
         <v>176.89</v>
@@ -774,8 +798,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n">
-        <v>45065</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2023-05-19 00:00:00</t>
+        </is>
       </c>
       <c r="B16" t="n">
         <v>180.14</v>
@@ -798,8 +824,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="n">
-        <v>45068</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-05-22 00:00:00</t>
+        </is>
       </c>
       <c r="B17" t="n">
         <v>188.87</v>
@@ -822,8 +850,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="n">
-        <v>45069</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-05-23 00:00:00</t>
+        </is>
       </c>
       <c r="B18" t="n">
         <v>185.77</v>
@@ -846,8 +876,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="n">
-        <v>45070</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2023-05-24 00:00:00</t>
+        </is>
       </c>
       <c r="B19" t="n">
         <v>182.9</v>
@@ -870,8 +902,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="n">
-        <v>45071</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2023-05-25 00:00:00</t>
+        </is>
       </c>
       <c r="B20" t="n">
         <v>184.47</v>
@@ -894,8 +928,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="n">
-        <v>45072</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2023-05-26 00:00:00</t>
+        </is>
       </c>
       <c r="B21" t="n">
         <v>193.17</v>
@@ -918,8 +954,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="n">
-        <v>45076</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2023-05-30 00:00:00</t>
+        </is>
       </c>
       <c r="B22" t="n">
         <v>201.16</v>
@@ -942,8 +980,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="n">
-        <v>45077</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2023-05-31 00:00:00</t>
+        </is>
       </c>
       <c r="B23" t="n">
         <v>203.93</v>
@@ -966,8 +1006,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="n">
-        <v>45413</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-05-01 00:00:00</t>
+        </is>
       </c>
       <c r="B24" t="n">
         <v>179.99</v>
@@ -990,8 +1032,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="n">
-        <v>45414</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-05-02 00:00:00</t>
+        </is>
       </c>
       <c r="B25" t="n">
         <v>180.01</v>
@@ -1014,8 +1058,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n">
-        <v>45415</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-05-03 00:00:00</t>
+        </is>
       </c>
       <c r="B26" t="n">
         <v>181.19</v>
@@ -1038,8 +1084,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="n">
-        <v>45418</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-05-06 00:00:00</t>
+        </is>
       </c>
       <c r="B27" t="n">
         <v>184.76</v>
@@ -1062,8 +1110,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="n">
-        <v>45419</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-05-07 00:00:00</t>
+        </is>
       </c>
       <c r="B28" t="n">
         <v>177.81</v>
@@ -1086,8 +1136,10 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="n">
-        <v>45420</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-05-08 00:00:00</t>
+        </is>
       </c>
       <c r="B29" t="n">
         <v>174.72</v>
@@ -1110,8 +1162,10 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="n">
-        <v>45421</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-05-09 00:00:00</t>
+        </is>
       </c>
       <c r="B30" t="n">
         <v>171.97</v>
@@ -1134,8 +1188,10 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="n">
-        <v>45422</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-05-10 00:00:00</t>
+        </is>
       </c>
       <c r="B31" t="n">
         <v>168.47</v>
@@ -1160,8 +1216,10 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="n">
-        <v>45425</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-05-13 00:00:00</t>
+        </is>
       </c>
       <c r="B32" t="n">
         <v>171.89</v>
@@ -1186,8 +1244,10 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="n">
-        <v>45426</v>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-05-14 00:00:00</t>
+        </is>
       </c>
       <c r="B33" t="n">
         <v>177.55</v>
@@ -1212,8 +1272,10 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="n">
-        <v>45427</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-05-15 00:00:00</t>
+        </is>
       </c>
       <c r="B34" t="n">
         <v>173.99</v>
@@ -1238,8 +1300,10 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="n">
-        <v>45428</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-05-16 00:00:00</t>
+        </is>
       </c>
       <c r="B35" t="n">
         <v>174.84</v>
@@ -1264,8 +1328,10 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="n">
-        <v>45429</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-05-17 00:00:00</t>
+        </is>
       </c>
       <c r="B36" t="n">
         <v>177.46</v>
@@ -1290,8 +1356,10 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="n">
-        <v>45432</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-05-20 00:00:00</t>
+        </is>
       </c>
       <c r="B37" t="n">
         <v>174.95</v>
@@ -1316,8 +1384,10 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="n">
-        <v>45433</v>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-05-21 00:00:00</t>
+        </is>
       </c>
       <c r="B38" t="n">
         <v>186.6</v>
@@ -1342,8 +1412,10 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="n">
-        <v>45434</v>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-05-22 00:00:00</t>
+        </is>
       </c>
       <c r="B39" t="n">
         <v>180.11</v>
@@ -1368,8 +1440,10 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="n">
-        <v>45435</v>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-05-23 00:00:00</t>
+        </is>
       </c>
       <c r="B40" t="n">
         <v>173.74</v>
@@ -1394,8 +1468,10 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="n">
-        <v>45436</v>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-05-24 00:00:00</t>
+        </is>
       </c>
       <c r="B41" t="n">
         <v>179.24</v>
@@ -1420,8 +1496,10 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="n">
-        <v>45440</v>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-05-28 00:00:00</t>
+        </is>
       </c>
       <c r="B42" t="n">
         <v>176.75</v>
@@ -1446,8 +1524,10 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="n">
-        <v>45441</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-05-29 00:00:00</t>
+        </is>
       </c>
       <c r="B43" t="n">
         <v>176.19</v>
@@ -1472,8 +1552,10 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="n">
-        <v>45442</v>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-05-30 00:00:00</t>
+        </is>
       </c>
       <c r="B44" t="n">
         <v>178.79</v>
@@ -1498,8 +1580,10 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="n">
-        <v>45443</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-05-31 00:00:00</t>
+        </is>
       </c>
       <c r="B45" t="n">
         <v>178.08</v>
@@ -1524,8 +1608,10 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="n">
-        <v>45778</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-05-01 00:00:00</t>
+        </is>
       </c>
       <c r="B46" t="n">
         <v>280.52</v>
@@ -1550,8 +1636,10 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="n">
-        <v>45779</v>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-05-02 00:00:00</t>
+        </is>
       </c>
       <c r="B47" t="n">
         <v>287.21</v>
@@ -1576,8 +1664,10 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="n">
-        <v>45782</v>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-05-05 00:00:00</t>
+        </is>
       </c>
       <c r="B48" t="n">
         <v>280.26</v>
@@ -1602,8 +1692,10 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="n">
-        <v>45783</v>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-05-06 00:00:00</t>
+        </is>
       </c>
       <c r="B49" t="n">
         <v>275.35</v>
@@ -1628,8 +1720,10 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="n">
-        <v>45784</v>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-05-07 00:00:00</t>
+        </is>
       </c>
       <c r="B50" t="n">
         <v>276.22</v>
@@ -1654,8 +1748,10 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="n">
-        <v>45785</v>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-05-08 00:00:00</t>
+        </is>
       </c>
       <c r="B51" t="n">
         <v>284.82</v>
@@ -1680,8 +1776,10 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="n">
-        <v>45786</v>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-05-09 00:00:00</t>
+        </is>
       </c>
       <c r="B52" t="n">
         <v>298.26</v>

</xml_diff>